<commit_message>
chore: Update master validation with evidence links
- All 29 features now have Evidence_links column populated
- Links point to EvidencePack/WinterRelease/TCO/ screenshots

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/WINTER_RELEASE_MASTER_VALIDATION.xlsx
+++ b/docs/WINTER_RELEASE_MASTER_VALIDATION.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm_r\intuit-boom\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5723F017-1733-4D6A-812F-C1C2E3FF117F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="294">
   <si>
     <t>Feature_id</t>
   </si>
@@ -722,6 +716,93 @@
   </si>
   <si>
     <t>Export</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-001_TCO_20251229_1102_UI_Accounting_AI_Banking.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-002_TCO_20251229_1102_UI_Sales_Tax_AI.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-003_TCO_20251229_1102_UI_Project_Management_AI.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-004_TCO_20251229_1102_UI_Homepage_Dashboard.png; EvidencePack/WinterRelease/TCO/WR-004_TCO_20251229_1103_UI_Finance_AI_Dashboard.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-005_TCO_20251229_1103_UI_Solutions_Specialist_Feed.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-006_TCO_20251229_1105_UI_Customer_Agent_Leads.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-007_TCO_20251229_1105_UI_Intuit_Intelligence.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-008_TCO_20251229_1105_UI_Conversational_BI.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-009_TCO_20251229_1102_UI_KPIs_Customizados.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-010_TCO_20251229_1102_UI_Dashboards.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-011_TCO_20251229_1105_UI_3P_Data_Integrations.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-012_TCO_20251229_1103_UI_Calculated_Fields_Reports.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-013_TCO_20251229_1103_UI_Management_Reports.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-014_TCO_20251229_1105_UI_Benchmarking.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-015_TCO_20251229_1103_UI_Multi_Entity_Reports.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-016_TCO_20251229_1102_UI_Dimension_Assignment.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-017_TCO_20251229_1103_UI_Hierarchical_Dimensions.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-018_TCO_20251229_1103_UI_Dimensions_Workflow.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-019_TCO_20251229_1103_UI_Dimensions_Balance_Sheet.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-020_TCO_20251229_1103_UI_Parallel_Approval.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-021_TCO_20251229_1105_UI_Desktop_Migration.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-022_TCO_20251229_1105_UI_DFY_Migration.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-023_TCO_20251229_1105_UI_Feature_Compatibility.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-024_TCO_20251229_1103_UI_Certified_Payroll.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-025_TCO_20251229_1105_UI_Sales_Order.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-026_TCO_20251229_1103_UI_Multi_Entity_Payroll.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-027_TCO_20251229_1105_UI_Garnishments.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-028_TCO_20251229_1105_UI_QBTime_Assignments.png</t>
+  </si>
+  <si>
+    <t>EvidencePack/WinterRelease/TCO/WR-029_TCO_20251229_1105_UI_Enhanced_Amendments.png</t>
   </si>
   <si>
     <t>Bank feed com sugestoes AI funcionando; Data: 434 rows</t>
@@ -820,8 +901,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -884,21 +965,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -936,7 +1009,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -970,7 +1043,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1005,10 +1077,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1181,35 +1252,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="59.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="101.6328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="78.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1315,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1305,14 +1355,17 @@
       <c r="M2" t="s">
         <v>230</v>
       </c>
+      <c r="N2" t="s">
+        <v>234</v>
+      </c>
       <c r="O2" t="s">
-        <v>234</v>
+        <v>263</v>
       </c>
       <c r="P2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1352,14 +1405,17 @@
       <c r="M3" t="s">
         <v>230</v>
       </c>
+      <c r="N3" t="s">
+        <v>235</v>
+      </c>
       <c r="O3" t="s">
-        <v>235</v>
+        <v>264</v>
       </c>
       <c r="P3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1399,14 +1455,17 @@
       <c r="M4" t="s">
         <v>230</v>
       </c>
+      <c r="N4" t="s">
+        <v>236</v>
+      </c>
       <c r="O4" t="s">
-        <v>236</v>
+        <v>265</v>
       </c>
       <c r="P4" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1446,14 +1505,17 @@
       <c r="M5" t="s">
         <v>231</v>
       </c>
+      <c r="N5" t="s">
+        <v>237</v>
+      </c>
       <c r="O5" t="s">
-        <v>237</v>
+        <v>266</v>
       </c>
       <c r="P5" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1493,14 +1555,17 @@
       <c r="M6" t="s">
         <v>231</v>
       </c>
+      <c r="N6" t="s">
+        <v>238</v>
+      </c>
       <c r="O6" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="P6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1540,14 +1605,17 @@
       <c r="M7" t="s">
         <v>231</v>
       </c>
+      <c r="N7" t="s">
+        <v>239</v>
+      </c>
       <c r="O7" t="s">
-        <v>239</v>
+        <v>268</v>
       </c>
       <c r="P7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1587,14 +1655,17 @@
       <c r="M8" t="s">
         <v>231</v>
       </c>
+      <c r="N8" t="s">
+        <v>240</v>
+      </c>
       <c r="O8" t="s">
-        <v>240</v>
+        <v>269</v>
       </c>
       <c r="P8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1634,14 +1705,17 @@
       <c r="M9" t="s">
         <v>231</v>
       </c>
+      <c r="N9" t="s">
+        <v>241</v>
+      </c>
       <c r="O9" t="s">
-        <v>241</v>
+        <v>270</v>
       </c>
       <c r="P9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1681,14 +1755,17 @@
       <c r="M10" t="s">
         <v>230</v>
       </c>
+      <c r="N10" t="s">
+        <v>242</v>
+      </c>
       <c r="O10" t="s">
-        <v>242</v>
+        <v>271</v>
       </c>
       <c r="P10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1728,14 +1805,17 @@
       <c r="M11" t="s">
         <v>231</v>
       </c>
+      <c r="N11" t="s">
+        <v>243</v>
+      </c>
       <c r="O11" t="s">
-        <v>243</v>
+        <v>272</v>
       </c>
       <c r="P11" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1775,14 +1855,17 @@
       <c r="M12" t="s">
         <v>231</v>
       </c>
+      <c r="N12" t="s">
+        <v>244</v>
+      </c>
       <c r="O12" t="s">
-        <v>244</v>
+        <v>273</v>
       </c>
       <c r="P12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1822,14 +1905,17 @@
       <c r="M13" t="s">
         <v>231</v>
       </c>
+      <c r="N13" t="s">
+        <v>245</v>
+      </c>
       <c r="O13" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
       <c r="P13" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1869,14 +1955,17 @@
       <c r="M14" t="s">
         <v>231</v>
       </c>
+      <c r="N14" t="s">
+        <v>246</v>
+      </c>
       <c r="O14" t="s">
-        <v>246</v>
+        <v>275</v>
       </c>
       <c r="P14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1916,14 +2005,17 @@
       <c r="M15" t="s">
         <v>231</v>
       </c>
+      <c r="N15" t="s">
+        <v>247</v>
+      </c>
       <c r="O15" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="P15" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1963,14 +2055,17 @@
       <c r="M16" t="s">
         <v>230</v>
       </c>
+      <c r="N16" t="s">
+        <v>248</v>
+      </c>
       <c r="O16" t="s">
-        <v>248</v>
+        <v>277</v>
       </c>
       <c r="P16" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2010,17 +2105,20 @@
       <c r="M17" t="s">
         <v>230</v>
       </c>
+      <c r="N17" t="s">
+        <v>249</v>
+      </c>
       <c r="O17" t="s">
-        <v>249</v>
+        <v>278</v>
       </c>
       <c r="P17" t="s">
-        <v>263</v>
+        <v>292</v>
       </c>
       <c r="Q17" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2060,14 +2158,17 @@
       <c r="M18" t="s">
         <v>230</v>
       </c>
+      <c r="N18" t="s">
+        <v>250</v>
+      </c>
       <c r="O18" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="P18" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2107,14 +2208,17 @@
       <c r="M19" t="s">
         <v>230</v>
       </c>
+      <c r="N19" t="s">
+        <v>251</v>
+      </c>
       <c r="O19" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
       <c r="P19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2154,14 +2258,17 @@
       <c r="M20" t="s">
         <v>231</v>
       </c>
+      <c r="N20" t="s">
+        <v>252</v>
+      </c>
       <c r="O20" t="s">
-        <v>252</v>
+        <v>281</v>
       </c>
       <c r="P20" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2201,14 +2308,17 @@
       <c r="M21" t="s">
         <v>232</v>
       </c>
+      <c r="N21" t="s">
+        <v>253</v>
+      </c>
       <c r="O21" t="s">
-        <v>253</v>
+        <v>282</v>
       </c>
       <c r="P21" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -2248,14 +2358,17 @@
       <c r="M22" t="s">
         <v>231</v>
       </c>
+      <c r="N22" t="s">
+        <v>254</v>
+      </c>
       <c r="O22" t="s">
-        <v>254</v>
+        <v>283</v>
       </c>
       <c r="P22" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2295,14 +2408,17 @@
       <c r="M23" t="s">
         <v>231</v>
       </c>
+      <c r="N23" t="s">
+        <v>255</v>
+      </c>
       <c r="O23" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
       <c r="P23" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2342,14 +2458,17 @@
       <c r="M24" t="s">
         <v>233</v>
       </c>
+      <c r="N24" t="s">
+        <v>256</v>
+      </c>
       <c r="O24" t="s">
-        <v>256</v>
+        <v>285</v>
       </c>
       <c r="P24" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2389,14 +2508,17 @@
       <c r="M25" t="s">
         <v>230</v>
       </c>
+      <c r="N25" t="s">
+        <v>257</v>
+      </c>
       <c r="O25" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="P25" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2436,14 +2558,17 @@
       <c r="M26" t="s">
         <v>231</v>
       </c>
+      <c r="N26" t="s">
+        <v>258</v>
+      </c>
       <c r="O26" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
       <c r="P26" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2483,14 +2608,17 @@
       <c r="M27" t="s">
         <v>230</v>
       </c>
+      <c r="N27" t="s">
+        <v>259</v>
+      </c>
       <c r="O27" t="s">
-        <v>259</v>
+        <v>288</v>
       </c>
       <c r="P27" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -2530,14 +2658,17 @@
       <c r="M28" t="s">
         <v>232</v>
       </c>
+      <c r="N28" t="s">
+        <v>260</v>
+      </c>
       <c r="O28" t="s">
-        <v>260</v>
+        <v>289</v>
       </c>
       <c r="P28" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -2577,14 +2708,17 @@
       <c r="M29" t="s">
         <v>230</v>
       </c>
+      <c r="N29" t="s">
+        <v>261</v>
+      </c>
       <c r="O29" t="s">
-        <v>261</v>
+        <v>290</v>
       </c>
       <c r="P29" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -2624,8 +2758,11 @@
       <c r="M30" t="s">
         <v>232</v>
       </c>
+      <c r="N30" t="s">
+        <v>262</v>
+      </c>
       <c r="O30" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
       <c r="P30" t="s">
         <v>172</v>

</xml_diff>

<commit_message>
consolidar: Winter Release TCO COMPLETO - SpineHub Deep
SESSAO COMPLETA:
- 29 screenshots validados (17 EXCELLENT, 8 GOOD, 4 N/A)
- Google Drive API configurada (OAuth2 + token persistente)
- Hyperlinks funcionais no tracker Excel
- Organizacao Drive: 06. Winter Release/TCO/

PROXIMO: Replicar para CONSTRUCTION

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/docs/WINTER_RELEASE_MASTER_VALIDATION.xlsx
+++ b/docs/WINTER_RELEASE_MASTER_VALIDATION.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adm_r\intuit-boom\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5945B8A-6ACD-4585-9669-352990C16406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -901,8 +907,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -965,13 +971,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1009,7 +1023,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1043,6 +1057,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1077,9 +1092,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1252,14 +1268,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="59.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="101.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="166.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="78.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1352,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1365,7 +1402,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1415,7 +1452,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1465,7 +1502,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1515,7 +1552,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1565,7 +1602,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1615,7 +1652,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1665,7 +1702,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1715,7 +1752,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1765,7 +1802,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1815,7 +1852,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1865,7 +1902,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1915,7 +1952,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1965,7 +2002,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2015,7 +2052,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -2065,7 +2102,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2118,7 +2155,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2168,7 +2205,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2218,7 +2255,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -2268,7 +2305,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2318,7 +2355,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -2368,7 +2405,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2418,7 +2455,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -2468,7 +2505,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -2518,7 +2555,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -2568,7 +2605,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -2618,7 +2655,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -2668,7 +2705,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -2718,7 +2755,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>46</v>
       </c>

</xml_diff>